<commit_message>
get expected return and risk
</commit_message>
<xml_diff>
--- a/correlation_matrix.xlsx
+++ b/correlation_matrix.xlsx
@@ -14,12 +14,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>S&amp;P500</t>
   </si>
   <si>
-    <t>EuroStoxx50</t>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Kospi200</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>WTI</t>
+  </si>
+  <si>
+    <t>K_treasury</t>
+  </si>
+  <si>
+    <t>K_corp_bond</t>
   </si>
   <si>
     <t>global_bonds</t>
@@ -380,13 +395,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -396,8 +411,23 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -405,37 +435,227 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.4626833985478638</v>
+        <v>0.6998666321284442</v>
       </c>
       <c r="D2">
-        <v>0.9202074331286239</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>0.8150783844262781</v>
+      </c>
+      <c r="E2">
+        <v>0.1156948483490844</v>
+      </c>
+      <c r="F2">
+        <v>-0.6037594671456528</v>
+      </c>
+      <c r="G2">
+        <v>0.784067051792052</v>
+      </c>
+      <c r="H2">
+        <v>0.7495275017817324</v>
+      </c>
+      <c r="I2">
+        <v>0.9202057654033214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.4626833985478638</v>
+        <v>0.6998666321284442</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.4011065760801188</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.8997079696946566</v>
+      </c>
+      <c r="E3">
+        <v>0.04379182799911028</v>
+      </c>
+      <c r="F3">
+        <v>-0.5314214205653955</v>
+      </c>
+      <c r="G3">
+        <v>0.6190401330723398</v>
+      </c>
+      <c r="H3">
+        <v>0.7153791319941667</v>
+      </c>
+      <c r="I3">
+        <v>0.5879142527021959</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.9202074331286239</v>
+        <v>0.8150783844262781</v>
       </c>
       <c r="C4">
-        <v>0.4011065760801188</v>
+        <v>0.8997079696946566</v>
       </c>
       <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>-0.1459691394944984</v>
+      </c>
+      <c r="F4">
+        <v>-0.5005338126282869</v>
+      </c>
+      <c r="G4">
+        <v>0.6707553186115066</v>
+      </c>
+      <c r="H4">
+        <v>0.7155247127037971</v>
+      </c>
+      <c r="I4">
+        <v>0.7020722691999959</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>0.1156948483490844</v>
+      </c>
+      <c r="C5">
+        <v>0.04379182799911028</v>
+      </c>
+      <c r="D5">
+        <v>-0.1459691394944984</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>-0.4834998051590432</v>
+      </c>
+      <c r="G5">
+        <v>0.1001054865159668</v>
+      </c>
+      <c r="H5">
+        <v>0.04754038645372555</v>
+      </c>
+      <c r="I5">
+        <v>0.1860429897050268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>-0.6037594671456528</v>
+      </c>
+      <c r="C6">
+        <v>-0.5314214205653955</v>
+      </c>
+      <c r="D6">
+        <v>-0.5005338126282869</v>
+      </c>
+      <c r="E6">
+        <v>-0.4834998051590432</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>-0.7454485727909008</v>
+      </c>
+      <c r="H6">
+        <v>-0.6810985214977375</v>
+      </c>
+      <c r="I6">
+        <v>-0.5322923581610045</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>0.784067051792052</v>
+      </c>
+      <c r="C7">
+        <v>0.6190401330723398</v>
+      </c>
+      <c r="D7">
+        <v>0.6707553186115066</v>
+      </c>
+      <c r="E7">
+        <v>0.1001054865159668</v>
+      </c>
+      <c r="F7">
+        <v>-0.7454485727909008</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>0.9182158444064913</v>
+      </c>
+      <c r="I7">
+        <v>0.6773559548205431</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>0.7495275017817324</v>
+      </c>
+      <c r="C8">
+        <v>0.7153791319941667</v>
+      </c>
+      <c r="D8">
+        <v>0.7155247127037971</v>
+      </c>
+      <c r="E8">
+        <v>0.04754038645372555</v>
+      </c>
+      <c r="F8">
+        <v>-0.6810985214977375</v>
+      </c>
+      <c r="G8">
+        <v>0.9182158444064913</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>0.6073162434477504</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>0.9202057654033214</v>
+      </c>
+      <c r="C9">
+        <v>0.5879142527021959</v>
+      </c>
+      <c r="D9">
+        <v>0.7020722691999959</v>
+      </c>
+      <c r="E9">
+        <v>0.1860429897050268</v>
+      </c>
+      <c r="F9">
+        <v>-0.5322923581610045</v>
+      </c>
+      <c r="G9">
+        <v>0.6773559548205431</v>
+      </c>
+      <c r="H9">
+        <v>0.6073162434477504</v>
+      </c>
+      <c r="I9">
         <v>1</v>
       </c>
     </row>

</xml_diff>